<commit_message>
All Testcases Running Fine
</commit_message>
<xml_diff>
--- a/Testcases/credential sheet.xlsx
+++ b/Testcases/credential sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="120">
   <si>
     <t>TestCase</t>
   </si>
@@ -88,6 +88,9 @@
     <t>Co_App_Downpay</t>
   </si>
   <si>
+    <t>Co_App_Gift_Description</t>
+  </si>
+  <si>
     <t>Co_App_Gift_assetvalue</t>
   </si>
   <si>
@@ -182,6 +185,9 @@
   </si>
   <si>
     <t>RRSP</t>
+  </si>
+  <si>
+    <t>Gift</t>
   </si>
   <si>
     <t>C128</t>
@@ -686,15 +692,15 @@
     <col customWidth="1" min="20" max="20" width="18.88"/>
     <col customWidth="1" min="21" max="21" width="21.5"/>
     <col customWidth="1" min="22" max="22" width="16.13"/>
-    <col customWidth="1" min="23" max="24" width="19.38"/>
-    <col customWidth="1" min="25" max="25" width="21.25"/>
-    <col customWidth="1" min="26" max="26" width="19.38"/>
-    <col customWidth="1" min="27" max="27" width="23.63"/>
-    <col customWidth="1" min="28" max="28" width="23.25"/>
-    <col customWidth="1" min="29" max="29" width="22.63"/>
-    <col customWidth="1" min="30" max="31" width="24.75"/>
-    <col customWidth="1" min="35" max="35" width="14.38"/>
-    <col customWidth="1" min="42" max="42" width="29.75"/>
+    <col customWidth="1" min="23" max="25" width="19.38"/>
+    <col customWidth="1" min="26" max="26" width="21.25"/>
+    <col customWidth="1" min="27" max="27" width="19.38"/>
+    <col customWidth="1" min="28" max="28" width="23.63"/>
+    <col customWidth="1" min="29" max="29" width="23.25"/>
+    <col customWidth="1" min="30" max="30" width="22.63"/>
+    <col customWidth="1" min="31" max="32" width="24.75"/>
+    <col customWidth="1" min="36" max="36" width="14.38"/>
+    <col customWidth="1" min="43" max="43" width="29.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -791,7 +797,7 @@
       <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
@@ -800,64 +806,67 @@
       <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" ht="26.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN2" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="AO2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -869,37 +878,37 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M4" s="1">
         <v>30000.0</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O4" s="6">
         <v>20000.0</v>
@@ -913,7 +922,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="W4" s="6">
         <v>20000.0</v>
@@ -921,47 +930,56 @@
       <c r="X4" s="6">
         <v>30000.0</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z4" s="6">
         <v>10000.0</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="AA4" s="6">
         <v>20000.0</v>
       </c>
-      <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="L5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="3">
+        <v>30000.0</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="O5" s="6">
         <v>20000.0</v>
       </c>
@@ -974,7 +992,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="W5" s="6">
         <v>20000.0</v>
@@ -982,61 +1000,62 @@
       <c r="X5" s="6">
         <v>30000.0</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
         <v>10000.0</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AA5" s="1">
         <v>20000.0</v>
       </c>
-      <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M6" s="1">
         <v>30000.0</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="O6" s="1">
         <v>100000.0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="1">
         <v>40000.0</v>
@@ -1049,65 +1068,68 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-      <c r="AA6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1" t="s">
+      <c r="Z6" s="6"/>
+      <c r="AB6" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="AC6" s="1">
+        <v>100000.0</v>
+      </c>
       <c r="AD6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE6" s="1">
+        <v>65</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF6" s="1">
         <v>50000.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M7" s="1">
         <v>30000.0</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="O7" s="1">
         <v>100000.0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q7" s="1">
         <v>40000.0</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T7" s="6">
         <v>20000.0</v>
@@ -1118,64 +1140,64 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="AF8" s="1">
+      <c r="AG8" s="1">
         <v>5000.0</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AH8" s="1">
         <v>500.0</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AI8" s="1">
         <v>1000.0</v>
       </c>
-      <c r="AI8" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="AJ8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK8" s="1">
+        <v>68</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL8" s="1">
         <v>7000.0</v>
       </c>
-      <c r="AL8" s="1">
+      <c r="AM8" s="1">
         <v>700.0</v>
       </c>
-      <c r="AM8" s="1">
+      <c r="AN8" s="1">
         <v>1000.0</v>
       </c>
-      <c r="AN8" s="5">
+      <c r="AO8" s="5">
         <v>44663.0</v>
       </c>
-      <c r="AO8" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="AP8" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AQ8" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13">
@@ -1188,6 +1210,7 @@
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
     </row>
     <row r="14">
       <c r="K14" s="3"/>
@@ -1239,43 +1262,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -1305,43 +1328,43 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E2" s="9">
         <v>16502.0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H2" s="7">
         <v>110.0</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L2" s="9">
         <v>16502.0</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -1371,16 +1394,16 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -1437,90 +1460,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1540,18 +1563,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>